<commit_message>
update file to send / error header temp
</commit_message>
<xml_diff>
--- a/Hardware/Bicycle_Project/Project Outputs for Bicycle_Project/BOM/Bicycle_Project.xlsx
+++ b/Hardware/Bicycle_Project/Project Outputs for Bicycle_Project/BOM/Bicycle_Project.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GUSTAVO\UNAL\Semestre_2024-1\Diseño_Digital\Digital-Desing\Hardware\Bicycle_Project\Project Outputs for Bicycle_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Developments\unal\2024-1S\Digital-Desing\Hardware\Bicycle_Project\Project Outputs for Bicycle_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{804A98B1-47E2-4C05-8BA6-13A49B466768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8CDF4A7A-8E47-4FA8-9E15-2DBE8C9911EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{7364FD04-4870-4597-9A68-2BD7C34CB8EF}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11835" xr2:uid="{640C0EE8-6315-4497-AC9B-324954EF79C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Bicycle_Project" sheetId="1" r:id="rId1"/>
@@ -30,8 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -194,22 +192,316 @@
     <t>C83060</t>
   </si>
   <si>
+    <t>CONN PWR JACK 2X5.5MM SOLDER</t>
+  </si>
+  <si>
+    <t>J202</t>
+  </si>
+  <si>
+    <t>HCTL</t>
+  </si>
+  <si>
+    <t>HC-DC-005-2.0T</t>
+  </si>
+  <si>
+    <t>C3010533</t>
+  </si>
+  <si>
+    <t>CONN RCPT USB2.0 MINI B SMD R/A</t>
+  </si>
+  <si>
+    <t>J200</t>
+  </si>
+  <si>
+    <t>EDAC Inc.</t>
+  </si>
+  <si>
+    <t>KH-MINI-SMT-5P-Cu</t>
+  </si>
+  <si>
+    <t>C2688795</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 40V 1A SOD123F</t>
+  </si>
+  <si>
+    <t>D200, D202, D203</t>
+  </si>
+  <si>
+    <t>Shanghai Prisemi Elec</t>
+  </si>
+  <si>
+    <t>PSBD1DF40V1H</t>
+  </si>
+  <si>
+    <t>C110730</t>
+  </si>
+  <si>
+    <t>IC FLASH 16M SPI 85MHZ 8SOP</t>
+  </si>
+  <si>
+    <t>U302</t>
+  </si>
+  <si>
+    <t>Zetta</t>
+  </si>
+  <si>
+    <t>ZD25WQ16BTIGR</t>
+  </si>
+  <si>
+    <t>C2896790</t>
+  </si>
+  <si>
+    <t>IC MCU 32BIT 64KB FLASH 48LQFP</t>
+  </si>
+  <si>
+    <t>U100</t>
+  </si>
+  <si>
+    <t>STMicroelectronics</t>
+  </si>
+  <si>
+    <t>STM32F030C8T6TR</t>
+  </si>
+  <si>
+    <t>C23922</t>
+  </si>
+  <si>
+    <t>IC USB TO UART BRIDGE QFN20</t>
+  </si>
+  <si>
+    <t>U300</t>
+  </si>
+  <si>
+    <t>Silicon Labs</t>
+  </si>
+  <si>
+    <t>CP2102N-A02-GQFN20R</t>
+  </si>
+  <si>
+    <t>C969913</t>
+  </si>
+  <si>
+    <t>LED GREEN CLEAR 0805 SMD</t>
+  </si>
+  <si>
+    <t>D301</t>
+  </si>
+  <si>
+    <t>XINGLIGHT</t>
+  </si>
+  <si>
+    <t>XL-2012UGC</t>
+  </si>
+  <si>
+    <t>C965815</t>
+  </si>
+  <si>
+    <t>LED RED CLEAR 0805 SMD</t>
+  </si>
+  <si>
+    <t>D201, D204, D300, D402</t>
+  </si>
+  <si>
+    <t>XL-2012SURC</t>
+  </si>
+  <si>
+    <t>C965812</t>
+  </si>
+  <si>
+    <t>MOSFET N-CH 20V SOT23</t>
+  </si>
+  <si>
+    <t>Q400, Q401, Q402, Q403, Q404, Q405, Q406, Q407</t>
+  </si>
+  <si>
+    <t>Doeshare</t>
+  </si>
+  <si>
+    <t>DN2302S</t>
+  </si>
+  <si>
+    <t>C2931750</t>
+  </si>
+  <si>
+    <t>RES SMD 1k OHM 5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>R403, R404, R405, R409, R414, R415, R416, R420, R421, R422, R428</t>
+  </si>
+  <si>
+    <t>FRC0603J102 TS</t>
+  </si>
+  <si>
+    <t>C2907113</t>
+  </si>
+  <si>
+    <t>RES SMD 4k7 OHM 5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>R426</t>
+  </si>
+  <si>
+    <t>FRC0603J472 TS</t>
+  </si>
+  <si>
+    <t>C2907166</t>
+  </si>
+  <si>
+    <t>RES SMD 5k1 OHM 5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>R101, R300</t>
+  </si>
+  <si>
+    <t>FRC0603J512 TS</t>
+  </si>
+  <si>
+    <t>C2907114</t>
+  </si>
+  <si>
+    <t>RES SMD 10k OHM 5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>R100, R102, R301, R304, R306, R307, R308, R309, R310, R311, R406, R407, R408, R410, R417, R418, R419, R423, R424, R425, R429</t>
+  </si>
+  <si>
+    <t>FRC0603J103TS</t>
+  </si>
+  <si>
+    <t>C2930027</t>
+  </si>
+  <si>
+    <t>RES SMD 24R OHM 5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>R401, R412</t>
+  </si>
+  <si>
+    <t>FRC0603J240 TS</t>
+  </si>
+  <si>
+    <t>C2907132</t>
+  </si>
+  <si>
+    <t>RES SMD 30R OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>R402, R413</t>
+  </si>
+  <si>
+    <t>FRC0603F30R0TS</t>
+  </si>
+  <si>
+    <t>C2907026</t>
+  </si>
+  <si>
+    <t>RES SMD 33R OHM 5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>R303</t>
+  </si>
+  <si>
+    <t>FRC0603J330 TS</t>
+  </si>
+  <si>
+    <t>C2907154</t>
+  </si>
+  <si>
+    <t>RES SMD 52R3 OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>R400, R411</t>
+  </si>
+  <si>
+    <t>FRC0603F52R3TS</t>
+  </si>
+  <si>
+    <t>C2998074</t>
+  </si>
+  <si>
+    <t>RES SMD 100R OHM 5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>R201, R302, R427</t>
+  </si>
+  <si>
+    <t>FRC0603J101 TS</t>
+  </si>
+  <si>
+    <t>C2907089</t>
+  </si>
+  <si>
+    <t>RES SMD 220R OHM 5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>R200</t>
+  </si>
+  <si>
+    <t>FRC0603J221 TS</t>
+  </si>
+  <si>
+    <t>C2907127</t>
+  </si>
+  <si>
+    <t>SWITCH TACTILE SPST-NO 0.05A 12V</t>
+  </si>
+  <si>
+    <t>SW100, SW400, SW401, SW402</t>
+  </si>
+  <si>
+    <t>BZCN</t>
+  </si>
+  <si>
+    <t>TSC015A05026A</t>
+  </si>
+  <si>
+    <t>C2888509</t>
+  </si>
+  <si>
+    <t>TVS DIODE 5.25V 17V SOT23-6</t>
+  </si>
+  <si>
+    <t>U301</t>
+  </si>
+  <si>
+    <t>USBLC6-2SC6</t>
+  </si>
+  <si>
+    <t>C7519</t>
+  </si>
+  <si>
+    <t>1A 60dB@(120Hz) Fixed 3.3V Positive 18V SOT-223 Linear Voltage Regulators (LDO) ROHS</t>
+  </si>
+  <si>
+    <t>U200</t>
+  </si>
+  <si>
+    <t>UMW(Youtai Semiconductor Co., Ltd.)</t>
+  </si>
+  <si>
+    <t>AMS1117-3.3</t>
+  </si>
+  <si>
+    <t>C347222</t>
+  </si>
+  <si>
     <t>CONN HEADER VERT 2POS 2.54MM</t>
   </si>
   <si>
     <t>J400</t>
   </si>
   <si>
-    <t>Samtec Inc.</t>
-  </si>
-  <si>
-    <t>TS-102-T-A</t>
-  </si>
-  <si>
-    <t>DigiKey</t>
-  </si>
-  <si>
-    <t>SAM1112-02-ND</t>
+    <t>Amphenol ICC (FCI)</t>
+  </si>
+  <si>
+    <t>10129378-902001BLF</t>
+  </si>
+  <si>
+    <t>Digi-Key</t>
+  </si>
+  <si>
+    <t>10129378-902001BLF-ND</t>
   </si>
   <si>
     <t>CONN HEADER VERT 3POS 2.54MM</t>
@@ -218,10 +510,10 @@
     <t>J402</t>
   </si>
   <si>
-    <t>TS-103-T-A</t>
-  </si>
-  <si>
-    <t>SAM1112-03-ND</t>
+    <t>10129378-903001BLF</t>
+  </si>
+  <si>
+    <t>10129378-903001BLF-ND</t>
   </si>
   <si>
     <t>CONN HEADER VERT 4POS 2.54MM</t>
@@ -230,10 +522,10 @@
     <t>J401</t>
   </si>
   <si>
-    <t>TS-104-T-A</t>
-  </si>
-  <si>
-    <t>SAM1112-04-ND</t>
+    <t>10129378-904001BLF</t>
+  </si>
+  <si>
+    <t>10129378-904001BLF-ND</t>
   </si>
   <si>
     <t>CONN HEADER VERT 5POS 2.54MM</t>
@@ -242,10 +534,10 @@
     <t>J100</t>
   </si>
   <si>
-    <t>TS-105-T-A</t>
-  </si>
-  <si>
-    <t>SAM1112-05-ND</t>
+    <t>10129378-905001BLF</t>
+  </si>
+  <si>
+    <t>10129378-905001BLF-ND</t>
   </si>
   <si>
     <t>CONN HEADER VERT 24POS 2.54MM</t>
@@ -254,304 +546,10 @@
     <t>J203</t>
   </si>
   <si>
-    <t>TD-112-T-A</t>
-  </si>
-  <si>
-    <t>SAM1114-12-ND</t>
-  </si>
-  <si>
-    <t>CONN PWR JACK 2X5.5MM SOLDER</t>
-  </si>
-  <si>
-    <t>J202</t>
-  </si>
-  <si>
-    <t>HCTL</t>
-  </si>
-  <si>
-    <t>HC-DC-005-2.0T</t>
-  </si>
-  <si>
-    <t>C3010533</t>
-  </si>
-  <si>
-    <t>CONN RCPT USB2.0 MINI B SMD R/A</t>
-  </si>
-  <si>
-    <t>J200</t>
-  </si>
-  <si>
-    <t>EDAC Inc.</t>
-  </si>
-  <si>
-    <t>KH-MINI-SMT-5P-Cu</t>
-  </si>
-  <si>
-    <t>C2688795</t>
-  </si>
-  <si>
-    <t>DIODE SCHOTTKY 40V 1A SOD123F</t>
-  </si>
-  <si>
-    <t>D200, D202, D203</t>
-  </si>
-  <si>
-    <t>Shanghai Prisemi Elec</t>
-  </si>
-  <si>
-    <t>PSBD1DF40V1H</t>
-  </si>
-  <si>
-    <t>C110730</t>
-  </si>
-  <si>
-    <t>IC FLASH 16M SPI 85MHZ 8SOP</t>
-  </si>
-  <si>
-    <t>U302</t>
-  </si>
-  <si>
-    <t>Zetta</t>
-  </si>
-  <si>
-    <t>ZD25WQ16BTIGR</t>
-  </si>
-  <si>
-    <t>C2896790</t>
-  </si>
-  <si>
-    <t>IC MCU 32BIT 64KB FLASH 48LQFP</t>
-  </si>
-  <si>
-    <t>U100</t>
-  </si>
-  <si>
-    <t>STMicroelectronics</t>
-  </si>
-  <si>
-    <t>STM32F030C8T6TR</t>
-  </si>
-  <si>
-    <t>C23922</t>
-  </si>
-  <si>
-    <t>IC USB TO UART BRIDGE QFN20</t>
-  </si>
-  <si>
-    <t>U300</t>
-  </si>
-  <si>
-    <t>Silicon Labs</t>
-  </si>
-  <si>
-    <t>CP2102N-A02-GQFN20R</t>
-  </si>
-  <si>
-    <t>C969913</t>
-  </si>
-  <si>
-    <t>LED GREEN CLEAR 0805 SMD</t>
-  </si>
-  <si>
-    <t>D301</t>
-  </si>
-  <si>
-    <t>XINGLIGHT</t>
-  </si>
-  <si>
-    <t>XL-2012UGC</t>
-  </si>
-  <si>
-    <t>C965815</t>
-  </si>
-  <si>
-    <t>LED RED CLEAR 0805 SMD</t>
-  </si>
-  <si>
-    <t>D201, D204, D300, D402</t>
-  </si>
-  <si>
-    <t>XL-2012SURC</t>
-  </si>
-  <si>
-    <t>C965812</t>
-  </si>
-  <si>
-    <t>MOSFET N-CH 20V SOT23</t>
-  </si>
-  <si>
-    <t>Q400, Q401, Q402, Q403, Q404, Q405, Q406, Q407</t>
-  </si>
-  <si>
-    <t>Doeshare</t>
-  </si>
-  <si>
-    <t>DN2302S</t>
-  </si>
-  <si>
-    <t>C2931750</t>
-  </si>
-  <si>
-    <t>RES SMD 1k OHM 5% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>R403, R404, R405, R409, R414, R415, R416, R420, R421, R422, R428</t>
-  </si>
-  <si>
-    <t>FRC0603J102 TS</t>
-  </si>
-  <si>
-    <t>C2907113</t>
-  </si>
-  <si>
-    <t>RES SMD 4k7 OHM 5% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>R426</t>
-  </si>
-  <si>
-    <t>FRC0603J472 TS</t>
-  </si>
-  <si>
-    <t>C2907166</t>
-  </si>
-  <si>
-    <t>RES SMD 5k1 OHM 5% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>R101, R300</t>
-  </si>
-  <si>
-    <t>FRC0603J512 TS</t>
-  </si>
-  <si>
-    <t>C2907114</t>
-  </si>
-  <si>
-    <t>RES SMD 10k OHM 5% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>R100, R102, R301, R304, R306, R307, R308, R309, R310, R311, R406, R407, R408, R410, R417, R418, R419, R423, R424, R425, R429</t>
-  </si>
-  <si>
-    <t>FRC0603J103TS</t>
-  </si>
-  <si>
-    <t>C2930027</t>
-  </si>
-  <si>
-    <t>RES SMD 24R OHM 5% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>R401, R412</t>
-  </si>
-  <si>
-    <t>FRC0603J240 TS</t>
-  </si>
-  <si>
-    <t>C2907132</t>
-  </si>
-  <si>
-    <t>RES SMD 30R OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>R402, R413</t>
-  </si>
-  <si>
-    <t>FRC0603F30R0TS</t>
-  </si>
-  <si>
-    <t>C2907026</t>
-  </si>
-  <si>
-    <t>RES SMD 33R OHM 5% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>R303</t>
-  </si>
-  <si>
-    <t>FRC0603J330 TS</t>
-  </si>
-  <si>
-    <t>C2907154</t>
-  </si>
-  <si>
-    <t>RES SMD 52R3 OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>R400, R411</t>
-  </si>
-  <si>
-    <t>FRC0603F52R3TS</t>
-  </si>
-  <si>
-    <t>C2998074</t>
-  </si>
-  <si>
-    <t>RES SMD 100R OHM 5% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>R201, R302, R427</t>
-  </si>
-  <si>
-    <t>FRC0603J101 TS</t>
-  </si>
-  <si>
-    <t>C2907089</t>
-  </si>
-  <si>
-    <t>RES SMD 220R OHM 5% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>R200</t>
-  </si>
-  <si>
-    <t>FRC0603J221 TS</t>
-  </si>
-  <si>
-    <t>C2907127</t>
-  </si>
-  <si>
-    <t>SWITCH TACTILE SPST-NO 0.05A 12V</t>
-  </si>
-  <si>
-    <t>SW100, SW400, SW401, SW402</t>
-  </si>
-  <si>
-    <t>BZCN</t>
-  </si>
-  <si>
-    <t>TSC015A05026A</t>
-  </si>
-  <si>
-    <t>C2888509</t>
-  </si>
-  <si>
-    <t>TVS DIODE 5.25V 17V SOT23-6</t>
-  </si>
-  <si>
-    <t>U301</t>
-  </si>
-  <si>
-    <t>USBLC6-2SC6</t>
-  </si>
-  <si>
-    <t>C7519</t>
-  </si>
-  <si>
-    <t>1A 60dB@(120Hz) Fixed 3.3V Positive 18V SOT-223 Linear Voltage Regulators (LDO) ROHS</t>
-  </si>
-  <si>
-    <t>U200</t>
-  </si>
-  <si>
-    <t>UMW(Youtai Semiconductor Co., Ltd.)</t>
-  </si>
-  <si>
-    <t>AMS1117-3.3</t>
-  </si>
-  <si>
-    <t>C347222</t>
+    <t>10129381-924001BLF</t>
+  </si>
+  <si>
+    <t>10129381-924001BLF-ND</t>
   </si>
 </sst>
 </file>
@@ -562,7 +560,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -632,7 +630,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -642,39 +640,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="156082"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -726,7 +724,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -837,6 +835,13 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -845,13 +850,6 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -916,47 +914,27 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1896944E-C5E2-4CF5-958E-57E318E676A9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9EF0380-2744-4175-8284-B01D469B69B4}">
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="7" width="16.5703125" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" customWidth="1"/>
+    <col min="1" max="2" width="20" customWidth="1"/>
+    <col min="3" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1231,10 +1209,10 @@
         <v>54</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1">
@@ -1243,19 +1221,19 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>59</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>60</v>
@@ -1273,40 +1251,42 @@
         <v>62</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="G13" s="1"/>
+        <v>65</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="H13" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1">
@@ -1315,22 +1295,22 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1">
@@ -1339,22 +1319,22 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1">
@@ -1363,22 +1343,22 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1">
@@ -1387,87 +1367,91 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="D18" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>25</v>
       </c>
       <c r="H18" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G19" s="1"/>
+        <v>94</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="H19" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>95</v>
+        <v>17</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="G20" s="1"/>
+        <v>98</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="H20" s="1">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>100</v>
+        <v>17</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>101</v>
@@ -1491,118 +1475,120 @@
         <v>104</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G22" s="1"/>
+      <c r="G22" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="H22" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>25</v>
       </c>
       <c r="H23" s="1">
-        <v>4</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="E24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>116</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>25</v>
       </c>
       <c r="H24" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>25</v>
       </c>
       <c r="H25" s="1">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1">
@@ -1611,22 +1597,22 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>25</v>
@@ -1637,100 +1623,98 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>25</v>
       </c>
       <c r="H28" s="1">
-        <v>21</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>25</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="G29" s="1"/>
       <c r="H29" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" s="2" t="s">
+      <c r="E30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>25</v>
       </c>
       <c r="H30" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D31" s="2" t="s">
+      <c r="E31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>144</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1">
@@ -1739,13 +1723,13 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>147</v>
@@ -1756,11 +1740,9 @@
       <c r="F32" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="G32" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="G32" s="1"/>
       <c r="H32" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1771,42 +1753,40 @@
         <v>150</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>17</v>
+        <v>151</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>12</v>
+        <v>153</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>25</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="G33" s="1"/>
       <c r="H33" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="F34" s="2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1">
@@ -1815,48 +1795,46 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>12</v>
+        <v>153</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>25</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="G35" s="1"/>
       <c r="H35" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>95</v>
+        <v>151</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>12</v>
+        <v>153</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="1">
@@ -1865,19 +1843,19 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>169</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>12</v>
+        <v>153</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>170</v>
@@ -1889,6 +1867,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
file to send delivery
</commit_message>
<xml_diff>
--- a/Hardware/Bicycle_Project/Project Outputs for Bicycle_Project/BOM/Bicycle_Project.xlsx
+++ b/Hardware/Bicycle_Project/Project Outputs for Bicycle_Project/BOM/Bicycle_Project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Developments\unal\2024-1S\Digital-Desing\Hardware\Bicycle_Project\Project Outputs for Bicycle_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8CDF4A7A-8E47-4FA8-9E15-2DBE8C9911EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3ED7D6FC-22BF-4E3A-831D-7048A3185D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11835" xr2:uid="{640C0EE8-6315-4497-AC9B-324954EF79C6}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11835" xr2:uid="{E787666E-2DCA-4969-85D9-F135C59EEC91}"/>
   </bookViews>
   <sheets>
     <sheet name="Bicycle_Project" sheetId="1" r:id="rId1"/>
@@ -925,7 +925,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9EF0380-2744-4175-8284-B01D469B69B4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{835CAA58-7496-4505-9BC2-2DE291E0B37D}">
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>